<commit_message>
no act version, please carefully check it
</commit_message>
<xml_diff>
--- a/design/design.xlsx
+++ b/design/design.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
-  <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/you/git/arch8/design/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14235" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="0.指令系统定义" sheetId="2" r:id="rId1"/>
@@ -19,11 +14,11 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -918,7 +913,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -961,7 +956,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -983,6 +978,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1273,13 +1271,13 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="55.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="49.33203125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="22.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="55.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="49.375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1452,15 +1450,15 @@
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="1"/>
-    <col min="4" max="4" width="67.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="8.875" style="1"/>
+    <col min="2" max="2" width="13.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.875" style="1"/>
+    <col min="4" max="4" width="67.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.875" style="1"/>
     <col min="6" max="6" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="1"/>
+    <col min="7" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
@@ -1828,18 +1826,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E68"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="3"/>
-    <col min="2" max="2" width="21.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="3"/>
+    <col min="2" max="2" width="21.625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" style="3" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="8.83203125" style="3"/>
+    <col min="6" max="16384" width="8.875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.2">
@@ -1857,7 +1855,7 @@
       </c>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>83</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1871,7 +1869,7 @@
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="8"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="3" t="s">
         <v>85</v>
       </c>
@@ -1883,7 +1881,7 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="8"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="3" t="s">
         <v>86</v>
       </c>
@@ -1923,7 +1921,7 @@
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>98</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1937,7 +1935,7 @@
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="8"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="3" t="s">
         <v>101</v>
       </c>
@@ -1949,10 +1947,10 @@
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="9" t="s">
         <v>142</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -1963,8 +1961,8 @@
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
       <c r="D14" s="3" t="s">
         <v>105</v>
       </c>
@@ -1973,10 +1971,10 @@
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="9" t="s">
         <v>115</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -1987,8 +1985,8 @@
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
       <c r="D17" s="3" t="s">
         <v>108</v>
       </c>
@@ -1997,8 +1995,8 @@
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
       <c r="D18" s="3" t="s">
         <v>109</v>
       </c>
@@ -2007,8 +2005,8 @@
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
       <c r="D19" s="3" t="s">
         <v>110</v>
       </c>
@@ -2017,8 +2015,8 @@
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
       <c r="D20" s="3" t="s">
         <v>111</v>
       </c>
@@ -2027,8 +2025,8 @@
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
       <c r="D21" s="3" t="s">
         <v>112</v>
       </c>
@@ -2037,8 +2035,8 @@
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
       <c r="D22" s="3" t="s">
         <v>113</v>
       </c>
@@ -2047,8 +2045,8 @@
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
       <c r="D23" s="3" t="s">
         <v>114</v>
       </c>
@@ -2057,10 +2055,10 @@
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="9" t="s">
         <v>126</v>
       </c>
       <c r="D25" s="3">
@@ -2071,8 +2069,8 @@
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
       <c r="D26" s="3" t="s">
         <v>125</v>
       </c>
@@ -2081,8 +2079,8 @@
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
       <c r="D27" s="3" t="s">
         <v>127</v>
       </c>
@@ -2091,8 +2089,8 @@
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
       <c r="D28" s="3">
         <v>1</v>
       </c>
@@ -2130,10 +2128,10 @@
     </row>
     <row r="33" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="9" t="s">
         <v>203</v>
       </c>
       <c r="D34" s="3" t="s">
@@ -2144,8 +2142,8 @@
       </c>
     </row>
     <row r="35" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
       <c r="D35" s="4" t="s">
         <v>205</v>
       </c>
@@ -2154,8 +2152,8 @@
       </c>
     </row>
     <row r="36" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
       <c r="D36" s="4" t="s">
         <v>204</v>
       </c>
@@ -2164,8 +2162,8 @@
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
       <c r="D37" s="3" t="s">
         <v>210</v>
       </c>
@@ -2174,7 +2172,7 @@
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B38" s="8"/>
+      <c r="B38" s="9"/>
       <c r="C38" s="3" t="s">
         <v>137</v>
       </c>
@@ -2186,10 +2184,10 @@
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="9" t="s">
         <v>141</v>
       </c>
       <c r="D40" s="3" t="s">
@@ -2200,8 +2198,8 @@
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
       <c r="D41" s="3" t="s">
         <v>136</v>
       </c>
@@ -2210,8 +2208,8 @@
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
       <c r="D42" s="3" t="s">
         <v>145</v>
       </c>
@@ -2220,8 +2218,8 @@
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
       <c r="D43" s="3" t="s">
         <v>114</v>
       </c>
@@ -2230,7 +2228,7 @@
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B45" s="8" t="s">
+      <c r="B45" s="9" t="s">
         <v>146</v>
       </c>
       <c r="C45" s="3" t="s">
@@ -2244,7 +2242,7 @@
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B46" s="8"/>
+      <c r="B46" s="9"/>
       <c r="C46" s="3" t="s">
         <v>148</v>
       </c>
@@ -2256,10 +2254,10 @@
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B48" s="8" t="s">
+      <c r="B48" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C48" s="9" t="s">
         <v>152</v>
       </c>
       <c r="D48" s="3">
@@ -2270,8 +2268,8 @@
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
       <c r="D49" s="3" t="s">
         <v>153</v>
       </c>
@@ -2280,8 +2278,8 @@
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
       <c r="D50" s="3" t="s">
         <v>154</v>
       </c>
@@ -2290,8 +2288,8 @@
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
       <c r="D51" s="3" t="s">
         <v>155</v>
       </c>
@@ -2300,8 +2298,8 @@
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
       <c r="D52" s="3" t="s">
         <v>156</v>
       </c>
@@ -2310,8 +2308,8 @@
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
       <c r="D53" s="3">
         <v>1</v>
       </c>
@@ -2334,7 +2332,7 @@
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B57" s="8" t="s">
+      <c r="B57" s="9" t="s">
         <v>161</v>
       </c>
       <c r="C57" s="3" t="s">
@@ -2348,7 +2346,7 @@
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B58" s="8"/>
+      <c r="B58" s="9"/>
       <c r="C58" s="3" t="s">
         <v>163</v>
       </c>
@@ -2360,10 +2358,10 @@
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B60" s="8" t="s">
+      <c r="B60" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="C60" s="8" t="s">
+      <c r="C60" s="9" t="s">
         <v>168</v>
       </c>
       <c r="D60" s="3" t="s">
@@ -2374,8 +2372,8 @@
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B61" s="8"/>
-      <c r="C61" s="8"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="9"/>
       <c r="D61" s="3" t="s">
         <v>169</v>
       </c>
@@ -2384,8 +2382,8 @@
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
       <c r="D62" s="3" t="s">
         <v>170</v>
       </c>
@@ -2394,8 +2392,8 @@
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B63" s="8"/>
-      <c r="C63" s="8"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9"/>
       <c r="D63" s="3" t="s">
         <v>171</v>
       </c>
@@ -2404,8 +2402,8 @@
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B64" s="8"/>
-      <c r="C64" s="8"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="9"/>
       <c r="D64" s="3" t="s">
         <v>172</v>
       </c>
@@ -2414,8 +2412,8 @@
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B65" s="8"/>
-      <c r="C65" s="8"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="9"/>
       <c r="D65" s="3" t="s">
         <v>173</v>
       </c>
@@ -2424,7 +2422,7 @@
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B67" s="8" t="s">
+      <c r="B67" s="9" t="s">
         <v>212</v>
       </c>
       <c r="C67" s="3" t="s">
@@ -2438,7 +2436,7 @@
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B68" s="8"/>
+      <c r="B68" s="9"/>
       <c r="C68" s="3" t="s">
         <v>214</v>
       </c>
@@ -2451,11 +2449,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B34:B38"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="B16:B23"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="B67:B68"/>
     <mergeCell ref="C25:C28"/>
     <mergeCell ref="C16:C23"/>
@@ -2470,6 +2463,11 @@
     <mergeCell ref="C48:C53"/>
     <mergeCell ref="B48:B53"/>
     <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B34:B38"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="B16:B23"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2478,46 +2476,47 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH82"/>
+  <dimension ref="A1:AK82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G86" sqref="G86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="3"/>
-    <col min="2" max="2" width="51.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="3"/>
+    <col min="2" max="2" width="51.625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="3"/>
-    <col min="7" max="7" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.875" style="3"/>
     <col min="8" max="8" width="6.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="3.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="3.125" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="8.83203125" style="3"/>
-    <col min="16" max="16" width="7.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="8.875" style="3"/>
+    <col min="16" max="16" width="7.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.125" style="3" bestFit="1" customWidth="1"/>
     <col min="21" max="22" width="6.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="4.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="4.875" style="3" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="4.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="4.625" style="3" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="32" max="34" width="6.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="35" max="16384" width="8.83203125" style="3"/>
+    <col min="32" max="34" width="6.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="6.875" style="8" customWidth="1"/>
+    <col min="37" max="37" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="38" max="16384" width="8.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="4" t="s">
         <v>179</v>
@@ -2534,9 +2533,6 @@
       <c r="F1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>97</v>
-      </c>
       <c r="H1" s="4" t="s">
         <v>99</v>
       </c>
@@ -2618,8 +2614,11 @@
       <c r="AH1" s="4" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AK1" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
         <v>178</v>
@@ -2636,7 +2635,7 @@
       <c r="F2" s="4">
         <v>3</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="8">
         <v>4</v>
       </c>
       <c r="H2" s="4">
@@ -2720,8 +2719,11 @@
       <c r="AH2" s="4">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AK2" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
         <v>180</v>
@@ -2738,7 +2740,7 @@
       <c r="F3" s="4">
         <v>0</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="8">
         <v>0</v>
       </c>
       <c r="H3" s="4">
@@ -2822,8 +2824,11 @@
       <c r="AH3" s="4" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AK3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="C4" s="3">
         <v>1</v>
       </c>
@@ -2836,7 +2841,7 @@
       <c r="F4" s="3">
         <v>1</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="8">
         <v>1</v>
       </c>
       <c r="H4" s="3">
@@ -2920,11 +2925,14 @@
       <c r="AH4" s="3" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AK4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
@@ -2940,7 +2948,7 @@
       <c r="F6" s="4">
         <v>1</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="8">
         <v>1</v>
       </c>
       <c r="H6" s="4">
@@ -3024,11 +3032,14 @@
       <c r="AH6" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AK6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>37</v>
       </c>
@@ -3044,7 +3055,7 @@
       <c r="F8" s="4">
         <v>1</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="8">
         <v>1</v>
       </c>
       <c r="H8" s="4">
@@ -3128,8 +3139,11 @@
       <c r="AH8" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AK8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>38</v>
       </c>
@@ -3145,7 +3159,7 @@
       <c r="F9" s="4">
         <v>1</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="8">
         <v>1</v>
       </c>
       <c r="H9" s="4">
@@ -3229,8 +3243,11 @@
       <c r="AH9" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AK9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>39</v>
       </c>
@@ -3246,7 +3263,7 @@
       <c r="F10" s="4">
         <v>1</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="8">
         <v>1</v>
       </c>
       <c r="H10" s="4">
@@ -3330,11 +3347,14 @@
       <c r="AH10" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AK10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>37</v>
       </c>
@@ -3350,7 +3370,7 @@
       <c r="F12" s="4">
         <v>1</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="8">
         <v>1</v>
       </c>
       <c r="H12" s="4">
@@ -3434,8 +3454,11 @@
       <c r="AH12" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AK12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>38</v>
       </c>
@@ -3451,7 +3474,7 @@
       <c r="F13" s="4">
         <v>1</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="8">
         <v>1</v>
       </c>
       <c r="H13" s="4">
@@ -3535,8 +3558,11 @@
       <c r="AH13" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AK13" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>51</v>
       </c>
@@ -3552,7 +3578,7 @@
       <c r="F14" s="4">
         <v>1</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="8">
         <v>1</v>
       </c>
       <c r="H14" s="4">
@@ -3636,11 +3662,14 @@
       <c r="AH14" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AK14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>40</v>
       </c>
@@ -3656,7 +3685,7 @@
       <c r="F16" s="4">
         <v>1</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="8">
         <v>1</v>
       </c>
       <c r="H16" s="4">
@@ -3740,11 +3769,14 @@
       <c r="AH16" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>52</v>
       </c>
@@ -3760,7 +3792,7 @@
       <c r="F18" s="4">
         <v>1</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="8">
         <v>1</v>
       </c>
       <c r="H18" s="4">
@@ -3844,8 +3876,11 @@
       <c r="AH18" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK18" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>42</v>
       </c>
@@ -3861,7 +3896,7 @@
       <c r="F19" s="4">
         <v>1</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="8">
         <v>1</v>
       </c>
       <c r="H19" s="4">
@@ -3945,11 +3980,14 @@
       <c r="AH19" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK19" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>49</v>
       </c>
@@ -3965,7 +4003,7 @@
       <c r="F21" s="4">
         <v>1</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="8">
         <v>1</v>
       </c>
       <c r="H21" s="4">
@@ -4049,8 +4087,11 @@
       <c r="AH21" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK21" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>43</v>
       </c>
@@ -4066,8 +4107,8 @@
       <c r="F22" s="4">
         <v>1</v>
       </c>
-      <c r="G22" s="4">
-        <v>0</v>
+      <c r="G22" s="8">
+        <v>1</v>
       </c>
       <c r="H22" s="4">
         <v>0</v>
@@ -4150,11 +4191,14 @@
       <c r="AH22" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK22" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>49</v>
       </c>
@@ -4170,7 +4214,7 @@
       <c r="F24" s="4">
         <v>1</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="8">
         <v>1</v>
       </c>
       <c r="H24" s="4">
@@ -4254,8 +4298,11 @@
       <c r="AH24" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK24" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>50</v>
       </c>
@@ -4271,8 +4318,8 @@
       <c r="F25" s="4">
         <v>1</v>
       </c>
-      <c r="G25" s="4">
-        <v>0</v>
+      <c r="G25" s="8">
+        <v>1</v>
       </c>
       <c r="H25" s="4">
         <v>0</v>
@@ -4355,11 +4402,14 @@
       <c r="AH25" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK25" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>37</v>
       </c>
@@ -4375,7 +4425,7 @@
       <c r="F27" s="4">
         <v>1</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="8">
         <v>1</v>
       </c>
       <c r="H27" s="4">
@@ -4459,8 +4509,11 @@
       <c r="AH27" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK27" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>38</v>
       </c>
@@ -4476,7 +4529,7 @@
       <c r="F28" s="4">
         <v>1</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="8">
         <v>1</v>
       </c>
       <c r="H28" s="4">
@@ -4560,8 +4613,11 @@
       <c r="AH28" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK28" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>44</v>
       </c>
@@ -4577,7 +4633,7 @@
       <c r="F29" s="4">
         <v>1</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="8">
         <v>1</v>
       </c>
       <c r="H29" s="4">
@@ -4661,11 +4717,14 @@
       <c r="AH29" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK29" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B31" s="7" t="s">
         <v>45</v>
       </c>
@@ -4681,7 +4740,7 @@
       <c r="F31" s="4">
         <v>1</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31" s="8">
         <v>1</v>
       </c>
       <c r="H31" s="4">
@@ -4765,8 +4824,11 @@
       <c r="AH31" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK31" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>54</v>
       </c>
@@ -4782,7 +4844,7 @@
       <c r="F32" s="4">
         <v>0</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G32" s="8">
         <v>1</v>
       </c>
       <c r="H32" s="4">
@@ -4866,8 +4928,11 @@
       <c r="AH32" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AK32" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B33" s="7" t="s">
         <v>55</v>
       </c>
@@ -4883,8 +4948,8 @@
       <c r="F33" s="4">
         <v>1</v>
       </c>
-      <c r="G33" s="4">
-        <v>0</v>
+      <c r="G33" s="8">
+        <v>1</v>
       </c>
       <c r="H33" s="4">
         <v>1</v>
@@ -4967,8 +5032,11 @@
       <c r="AH33" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AK33" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>56</v>
       </c>
@@ -4984,7 +5052,7 @@
       <c r="F34" s="4">
         <v>0</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34" s="8">
         <v>1</v>
       </c>
       <c r="H34" s="4">
@@ -5068,8 +5136,11 @@
       <c r="AH34" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AK34" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>57</v>
       </c>
@@ -5085,8 +5156,8 @@
       <c r="F35" s="4">
         <v>1</v>
       </c>
-      <c r="G35" s="4">
-        <v>0</v>
+      <c r="G35" s="8">
+        <v>1</v>
       </c>
       <c r="H35" s="4">
         <v>1</v>
@@ -5169,8 +5240,11 @@
       <c r="AH35" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AK35" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>58</v>
       </c>
@@ -5186,7 +5260,7 @@
       <c r="F36" s="4">
         <v>1</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G36" s="8">
         <v>1</v>
       </c>
       <c r="H36" s="4">
@@ -5270,11 +5344,14 @@
       <c r="AH36" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AK36" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="1" t="s">
         <v>37</v>
@@ -5291,7 +5368,7 @@
       <c r="F38" s="4">
         <v>1</v>
       </c>
-      <c r="G38" s="4">
+      <c r="G38" s="8">
         <v>1</v>
       </c>
       <c r="H38" s="4">
@@ -5375,8 +5452,11 @@
       <c r="AH38" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AK38" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" s="1" t="s">
         <v>38</v>
@@ -5393,7 +5473,7 @@
       <c r="F39" s="4">
         <v>1</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G39" s="8">
         <v>1</v>
       </c>
       <c r="H39" s="4">
@@ -5477,8 +5557,11 @@
       <c r="AH39" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AK39" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>59</v>
       </c>
@@ -5494,7 +5577,7 @@
       <c r="F40" s="4">
         <v>1</v>
       </c>
-      <c r="G40" s="4">
+      <c r="G40" s="8">
         <v>1</v>
       </c>
       <c r="H40" s="4">
@@ -5578,8 +5661,11 @@
       <c r="AH40" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AK40" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
         <v>63</v>
       </c>
@@ -5595,7 +5681,7 @@
       <c r="F41" s="4">
         <v>1</v>
       </c>
-      <c r="G41" s="4">
+      <c r="G41" s="8">
         <v>1</v>
       </c>
       <c r="H41" s="4">
@@ -5679,8 +5765,11 @@
       <c r="AH41" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AK41" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>44</v>
       </c>
@@ -5696,7 +5785,7 @@
       <c r="F42" s="4">
         <v>1</v>
       </c>
-      <c r="G42" s="4">
+      <c r="G42" s="8">
         <v>1</v>
       </c>
       <c r="H42" s="4">
@@ -5780,11 +5869,14 @@
       <c r="AH42" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AK42" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
         <v>62</v>
       </c>
@@ -5800,7 +5892,7 @@
       <c r="F44" s="4">
         <v>1</v>
       </c>
-      <c r="G44" s="4">
+      <c r="G44" s="8">
         <v>1</v>
       </c>
       <c r="H44" s="4">
@@ -5884,8 +5976,11 @@
       <c r="AH44" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AK44" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
         <v>64</v>
       </c>
@@ -5901,7 +5996,7 @@
       <c r="F45" s="4">
         <v>1</v>
       </c>
-      <c r="G45" s="4">
+      <c r="G45" s="8">
         <v>1</v>
       </c>
       <c r="H45" s="4">
@@ -5985,8 +6080,11 @@
       <c r="AH45" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AK45" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
         <v>65</v>
       </c>
@@ -6002,7 +6100,7 @@
       <c r="F46" s="4">
         <v>1</v>
       </c>
-      <c r="G46" s="4">
+      <c r="G46" s="8">
         <v>1</v>
       </c>
       <c r="H46" s="4">
@@ -6086,8 +6184,11 @@
       <c r="AH46" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AK46" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
         <v>44</v>
       </c>
@@ -6103,7 +6204,7 @@
       <c r="F47" s="4">
         <v>1</v>
       </c>
-      <c r="G47" s="4">
+      <c r="G47" s="8">
         <v>1</v>
       </c>
       <c r="H47" s="4">
@@ -6187,11 +6288,14 @@
       <c r="AH47" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AK47" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B48" s="1"/>
     </row>
-    <row r="49" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
         <v>66</v>
       </c>
@@ -6207,7 +6311,7 @@
       <c r="F49" s="4">
         <v>1</v>
       </c>
-      <c r="G49" s="4">
+      <c r="G49" s="8">
         <v>1</v>
       </c>
       <c r="H49" s="4">
@@ -6291,11 +6395,14 @@
       <c r="AH49" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK49" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B50" s="1"/>
     </row>
-    <row r="51" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
         <v>67</v>
       </c>
@@ -6311,7 +6418,7 @@
       <c r="F51" s="4">
         <v>1</v>
       </c>
-      <c r="G51" s="4">
+      <c r="G51" s="8">
         <v>1</v>
       </c>
       <c r="H51" s="4">
@@ -6395,8 +6502,11 @@
       <c r="AH51" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK51" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
         <v>68</v>
       </c>
@@ -6412,7 +6522,7 @@
       <c r="F52" s="4">
         <v>1</v>
       </c>
-      <c r="G52" s="4">
+      <c r="G52" s="8">
         <v>1</v>
       </c>
       <c r="H52" s="4">
@@ -6496,11 +6606,14 @@
       <c r="AH52" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK52" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B53" s="1"/>
     </row>
-    <row r="54" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
         <v>71</v>
       </c>
@@ -6516,7 +6629,7 @@
       <c r="F54" s="4">
         <v>1</v>
       </c>
-      <c r="G54" s="4">
+      <c r="G54" s="8">
         <v>1</v>
       </c>
       <c r="H54" s="4">
@@ -6600,8 +6713,11 @@
       <c r="AH54" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK54" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B55" s="1" t="s">
         <v>69</v>
       </c>
@@ -6617,7 +6733,7 @@
       <c r="F55" s="4">
         <v>1</v>
       </c>
-      <c r="G55" s="4">
+      <c r="G55" s="8">
         <v>1</v>
       </c>
       <c r="H55" s="4">
@@ -6701,8 +6817,11 @@
       <c r="AH55" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK55" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B56" s="1" t="s">
         <v>70</v>
       </c>
@@ -6718,8 +6837,8 @@
       <c r="F56" s="4">
         <v>1</v>
       </c>
-      <c r="G56" s="4">
-        <v>0</v>
+      <c r="G56" s="8">
+        <v>1</v>
       </c>
       <c r="H56" s="4">
         <v>1</v>
@@ -6802,11 +6921,14 @@
       <c r="AH56" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK56" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B57" s="1"/>
     </row>
-    <row r="58" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B58" s="1" t="s">
         <v>72</v>
       </c>
@@ -6822,7 +6944,7 @@
       <c r="F58" s="4">
         <v>1</v>
       </c>
-      <c r="G58" s="4">
+      <c r="G58" s="8">
         <v>1</v>
       </c>
       <c r="H58" s="4">
@@ -6906,8 +7028,11 @@
       <c r="AH58" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK58" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B59" s="1" t="s">
         <v>73</v>
       </c>
@@ -6923,8 +7048,8 @@
       <c r="F59" s="4">
         <v>1</v>
       </c>
-      <c r="G59" s="4">
-        <v>0</v>
+      <c r="G59" s="8">
+        <v>1</v>
       </c>
       <c r="H59" s="4">
         <v>1</v>
@@ -7007,11 +7132,14 @@
       <c r="AH59" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK59" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B60" s="1"/>
     </row>
-    <row r="61" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B61" s="1" t="s">
         <v>37</v>
       </c>
@@ -7027,7 +7155,7 @@
       <c r="F61" s="4">
         <v>1</v>
       </c>
-      <c r="G61" s="4">
+      <c r="G61" s="8">
         <v>1</v>
       </c>
       <c r="H61" s="4">
@@ -7111,8 +7239,11 @@
       <c r="AH61" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK61" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B62" s="1" t="s">
         <v>74</v>
       </c>
@@ -7128,7 +7259,7 @@
       <c r="F62" s="4">
         <v>1</v>
       </c>
-      <c r="G62" s="4">
+      <c r="G62" s="8">
         <v>1</v>
       </c>
       <c r="H62" s="4">
@@ -7212,8 +7343,11 @@
       <c r="AH62" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK62" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B63" s="1" t="s">
         <v>75</v>
       </c>
@@ -7229,7 +7363,7 @@
       <c r="F63" s="4">
         <v>0</v>
       </c>
-      <c r="G63" s="4">
+      <c r="G63" s="8">
         <v>1</v>
       </c>
       <c r="H63" s="4">
@@ -7313,8 +7447,11 @@
       <c r="AH63" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK63" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B64" s="1" t="s">
         <v>76</v>
       </c>
@@ -7330,8 +7467,8 @@
       <c r="F64" s="4">
         <v>1</v>
       </c>
-      <c r="G64" s="4">
-        <v>0</v>
+      <c r="G64" s="8">
+        <v>1</v>
       </c>
       <c r="H64" s="4">
         <v>1</v>
@@ -7414,11 +7551,14 @@
       <c r="AH64" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK64" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B65" s="1"/>
     </row>
-    <row r="66" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B66" s="1" t="s">
         <v>45</v>
       </c>
@@ -7434,7 +7574,7 @@
       <c r="F66" s="4">
         <v>1</v>
       </c>
-      <c r="G66" s="4">
+      <c r="G66" s="8">
         <v>1</v>
       </c>
       <c r="H66" s="4">
@@ -7518,8 +7658,11 @@
       <c r="AH66" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK66" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
         <v>54</v>
       </c>
@@ -7535,7 +7678,7 @@
       <c r="F67" s="4">
         <v>0</v>
       </c>
-      <c r="G67" s="4">
+      <c r="G67" s="8">
         <v>1</v>
       </c>
       <c r="H67" s="4">
@@ -7619,8 +7762,11 @@
       <c r="AH67" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK67" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B68" s="7" t="s">
         <v>55</v>
       </c>
@@ -7636,8 +7782,8 @@
       <c r="F68" s="4">
         <v>1</v>
       </c>
-      <c r="G68" s="4">
-        <v>0</v>
+      <c r="G68" s="8">
+        <v>1</v>
       </c>
       <c r="H68" s="4">
         <v>1</v>
@@ -7720,8 +7866,11 @@
       <c r="AH68" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK68" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B69" s="1" t="s">
         <v>56</v>
       </c>
@@ -7737,7 +7886,7 @@
       <c r="F69" s="4">
         <v>0</v>
       </c>
-      <c r="G69" s="4">
+      <c r="G69" s="8">
         <v>1</v>
       </c>
       <c r="H69" s="4">
@@ -7821,8 +7970,11 @@
       <c r="AH69" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK69" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B70" s="1" t="s">
         <v>57</v>
       </c>
@@ -7838,8 +7990,8 @@
       <c r="F70" s="4">
         <v>1</v>
       </c>
-      <c r="G70" s="4">
-        <v>0</v>
+      <c r="G70" s="8">
+        <v>1</v>
       </c>
       <c r="H70" s="4">
         <v>1</v>
@@ -7922,8 +8074,11 @@
       <c r="AH70" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK70" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B71" s="1" t="s">
         <v>77</v>
       </c>
@@ -7939,7 +8094,7 @@
       <c r="F71" s="4">
         <v>1</v>
       </c>
-      <c r="G71" s="4">
+      <c r="G71" s="8">
         <v>1</v>
       </c>
       <c r="H71" s="4">
@@ -8023,11 +8178,14 @@
       <c r="AH71" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK71" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B72" s="1"/>
     </row>
-    <row r="73" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B73" s="1" t="s">
         <v>45</v>
       </c>
@@ -8043,7 +8201,7 @@
       <c r="F73" s="4">
         <v>1</v>
       </c>
-      <c r="G73" s="4">
+      <c r="G73" s="8">
         <v>1</v>
       </c>
       <c r="H73" s="4">
@@ -8127,8 +8285,11 @@
       <c r="AH73" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK73" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B74" s="1" t="s">
         <v>54</v>
       </c>
@@ -8144,7 +8305,7 @@
       <c r="F74" s="4">
         <v>0</v>
       </c>
-      <c r="G74" s="4">
+      <c r="G74" s="8">
         <v>1</v>
       </c>
       <c r="H74" s="4">
@@ -8228,8 +8389,11 @@
       <c r="AH74" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK74" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B75" s="7" t="s">
         <v>55</v>
       </c>
@@ -8245,8 +8409,8 @@
       <c r="F75" s="4">
         <v>1</v>
       </c>
-      <c r="G75" s="4">
-        <v>0</v>
+      <c r="G75" s="8">
+        <v>1</v>
       </c>
       <c r="H75" s="4">
         <v>1</v>
@@ -8329,8 +8493,11 @@
       <c r="AH75" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK75" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B76" s="1" t="s">
         <v>56</v>
       </c>
@@ -8346,7 +8513,7 @@
       <c r="F76" s="4">
         <v>0</v>
       </c>
-      <c r="G76" s="4">
+      <c r="G76" s="8">
         <v>1</v>
       </c>
       <c r="H76" s="4">
@@ -8430,8 +8597,11 @@
       <c r="AH76" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK76" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B77" s="1" t="s">
         <v>57</v>
       </c>
@@ -8447,8 +8617,8 @@
       <c r="F77" s="4">
         <v>1</v>
       </c>
-      <c r="G77" s="4">
-        <v>0</v>
+      <c r="G77" s="8">
+        <v>1</v>
       </c>
       <c r="H77" s="4">
         <v>1</v>
@@ -8531,8 +8701,11 @@
       <c r="AH77" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK77" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B78" s="1" t="s">
         <v>78</v>
       </c>
@@ -8548,7 +8721,7 @@
       <c r="F78" s="4">
         <v>1</v>
       </c>
-      <c r="G78" s="4">
+      <c r="G78" s="8">
         <v>1</v>
       </c>
       <c r="H78" s="4">
@@ -8632,11 +8805,14 @@
       <c r="AH78" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK78" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B79" s="1"/>
     </row>
-    <row r="80" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B80" s="1" t="s">
         <v>79</v>
       </c>
@@ -8652,7 +8828,7 @@
       <c r="F80" s="4">
         <v>1</v>
       </c>
-      <c r="G80" s="4">
+      <c r="G80" s="8">
         <v>1</v>
       </c>
       <c r="H80" s="4">
@@ -8736,8 +8912,11 @@
       <c r="AH80" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK80" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B81" s="1" t="s">
         <v>219</v>
       </c>
@@ -8753,7 +8932,7 @@
       <c r="F81" s="4">
         <v>1</v>
       </c>
-      <c r="G81" s="4">
+      <c r="G81" s="8">
         <v>1</v>
       </c>
       <c r="H81" s="4">
@@ -8837,8 +9016,11 @@
       <c r="AH81" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="AK81" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B82" s="1" t="s">
         <v>81</v>
       </c>
@@ -8854,8 +9036,8 @@
       <c r="F82" s="4">
         <v>1</v>
       </c>
-      <c r="G82" s="4">
-        <v>0</v>
+      <c r="G82" s="8">
+        <v>1</v>
       </c>
       <c r="H82" s="4">
         <v>1</v>
@@ -8936,11 +9118,15 @@
         <v>0</v>
       </c>
       <c r="AH82" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK82" s="4">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add control signal(hex version)
</commit_message>
<xml_diff>
--- a/design/design.xlsx
+++ b/design/design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14235" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="0.指令系统定义" sheetId="2" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="微操作信号表" sheetId="3" r:id="rId3"/>
     <sheet name="微指令控制操作对应表" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="266">
   <si>
     <t>LD Ai, addr</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1183,7 +1183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1223,6 +1223,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1506,8 +1509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:XFD43"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2399,7 +2402,7 @@
       </c>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="14" t="s">
         <v>77</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -2413,7 +2416,7 @@
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="11"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="3" t="s">
         <v>79</v>
       </c>
@@ -2425,7 +2428,7 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="11"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="3" t="s">
         <v>80</v>
       </c>
@@ -2465,7 +2468,7 @@
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="14" t="s">
         <v>92</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -2479,7 +2482,7 @@
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="11"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="3" t="s">
         <v>95</v>
       </c>
@@ -2491,10 +2494,10 @@
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="14" t="s">
         <v>136</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -2505,8 +2508,8 @@
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
       <c r="D14" s="3" t="s">
         <v>99</v>
       </c>
@@ -2515,10 +2518,10 @@
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="14" t="s">
         <v>109</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -2529,8 +2532,8 @@
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
       <c r="D17" s="3" t="s">
         <v>102</v>
       </c>
@@ -2539,8 +2542,8 @@
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="3" t="s">
         <v>103</v>
       </c>
@@ -2549,8 +2552,8 @@
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
       <c r="D19" s="3" t="s">
         <v>104</v>
       </c>
@@ -2559,8 +2562,8 @@
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
       <c r="D20" s="3" t="s">
         <v>105</v>
       </c>
@@ -2569,8 +2572,8 @@
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
       <c r="D21" s="3" t="s">
         <v>106</v>
       </c>
@@ -2579,8 +2582,8 @@
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
       <c r="D22" s="3" t="s">
         <v>107</v>
       </c>
@@ -2589,8 +2592,8 @@
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
       <c r="D23" s="3" t="s">
         <v>108</v>
       </c>
@@ -2599,10 +2602,10 @@
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="14" t="s">
         <v>120</v>
       </c>
       <c r="D25" s="3">
@@ -2613,8 +2616,8 @@
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
       <c r="D26" s="3" t="s">
         <v>119</v>
       </c>
@@ -2623,8 +2626,8 @@
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
       <c r="D27" s="3" t="s">
         <v>121</v>
       </c>
@@ -2633,8 +2636,8 @@
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
       <c r="D28" s="3">
         <v>1</v>
       </c>
@@ -2672,10 +2675,10 @@
     </row>
     <row r="33" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="14" t="s">
         <v>197</v>
       </c>
       <c r="D34" s="3" t="s">
@@ -2686,8 +2689,8 @@
       </c>
     </row>
     <row r="35" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
       <c r="D35" s="4" t="s">
         <v>199</v>
       </c>
@@ -2696,8 +2699,8 @@
       </c>
     </row>
     <row r="36" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
       <c r="D36" s="4" t="s">
         <v>198</v>
       </c>
@@ -2706,8 +2709,8 @@
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
       <c r="D37" s="3" t="s">
         <v>204</v>
       </c>
@@ -2716,7 +2719,7 @@
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B38" s="11"/>
+      <c r="B38" s="14"/>
       <c r="C38" s="3" t="s">
         <v>131</v>
       </c>
@@ -2728,10 +2731,10 @@
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="14" t="s">
         <v>135</v>
       </c>
       <c r="D40" s="3" t="s">
@@ -2742,8 +2745,8 @@
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
       <c r="D41" s="3" t="s">
         <v>130</v>
       </c>
@@ -2752,8 +2755,8 @@
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
       <c r="D42" s="3" t="s">
         <v>139</v>
       </c>
@@ -2762,8 +2765,8 @@
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
       <c r="D43" s="3" t="s">
         <v>108</v>
       </c>
@@ -2772,7 +2775,7 @@
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="14" t="s">
         <v>140</v>
       </c>
       <c r="C45" s="3" t="s">
@@ -2786,7 +2789,7 @@
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B46" s="11"/>
+      <c r="B46" s="14"/>
       <c r="C46" s="3" t="s">
         <v>142</v>
       </c>
@@ -2798,10 +2801,10 @@
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B48" s="11" t="s">
+      <c r="B48" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="14" t="s">
         <v>146</v>
       </c>
       <c r="D48" s="3">
@@ -2812,8 +2815,8 @@
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
       <c r="D49" s="3" t="s">
         <v>147</v>
       </c>
@@ -2822,8 +2825,8 @@
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
       <c r="D50" s="3" t="s">
         <v>148</v>
       </c>
@@ -2832,8 +2835,8 @@
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
       <c r="D51" s="3" t="s">
         <v>149</v>
       </c>
@@ -2842,8 +2845,8 @@
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
       <c r="D52" s="3" t="s">
         <v>150</v>
       </c>
@@ -2852,8 +2855,8 @@
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
       <c r="D53" s="3">
         <v>1</v>
       </c>
@@ -2876,7 +2879,7 @@
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B57" s="11" t="s">
+      <c r="B57" s="14" t="s">
         <v>155</v>
       </c>
       <c r="C57" s="3" t="s">
@@ -2890,7 +2893,7 @@
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B58" s="11"/>
+      <c r="B58" s="14"/>
       <c r="C58" s="3" t="s">
         <v>157</v>
       </c>
@@ -2902,10 +2905,10 @@
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B60" s="11" t="s">
+      <c r="B60" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="C60" s="11" t="s">
+      <c r="C60" s="14" t="s">
         <v>162</v>
       </c>
       <c r="D60" s="3" t="s">
@@ -2916,8 +2919,8 @@
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
       <c r="D61" s="3" t="s">
         <v>163</v>
       </c>
@@ -2926,8 +2929,8 @@
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B62" s="11"/>
-      <c r="C62" s="11"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
       <c r="D62" s="3" t="s">
         <v>164</v>
       </c>
@@ -2936,8 +2939,8 @@
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="14"/>
       <c r="D63" s="3" t="s">
         <v>165</v>
       </c>
@@ -2946,8 +2949,8 @@
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="14"/>
       <c r="D64" s="3" t="s">
         <v>166</v>
       </c>
@@ -2956,8 +2959,8 @@
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B65" s="11"/>
-      <c r="C65" s="11"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="14"/>
       <c r="D65" s="3" t="s">
         <v>167</v>
       </c>
@@ -2966,7 +2969,7 @@
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B67" s="11" t="s">
+      <c r="B67" s="14" t="s">
         <v>206</v>
       </c>
       <c r="C67" s="3" t="s">
@@ -2980,7 +2983,7 @@
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B68" s="11"/>
+      <c r="B68" s="14"/>
       <c r="C68" s="3" t="s">
         <v>208</v>
       </c>
@@ -2993,6 +2996,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B34:B38"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="B16:B23"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="B67:B68"/>
     <mergeCell ref="C25:C28"/>
     <mergeCell ref="C16:C23"/>
@@ -3007,11 +3015,6 @@
     <mergeCell ref="C48:C53"/>
     <mergeCell ref="B48:B53"/>
     <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B34:B38"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="B16:B23"/>
-    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3021,47 +3024,52 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK85"/>
+  <dimension ref="A1:AU85"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AI22" sqref="AI22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AR1" sqref="AR1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.875" style="3"/>
     <col min="2" max="2" width="51.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.875" style="3"/>
-    <col min="8" max="8" width="6.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="3.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="3.25" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="8.875" style="3"/>
-    <col min="16" max="16" width="7.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="6.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="4.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="4.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="32" max="34" width="6.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="6.875" style="8" customWidth="1"/>
-    <col min="37" max="37" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="38" max="16384" width="8.875" style="3"/>
+    <col min="14" max="15" width="9" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="6.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="5.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="32" max="34" width="7.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="5.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5.75" style="11" bestFit="1" customWidth="1"/>
+    <col min="37" max="42" width="5.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="44" max="46" width="5.75" style="11" customWidth="1"/>
+    <col min="47" max="47" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="48" max="16384" width="8.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="4" t="s">
         <v>173</v>
@@ -3159,11 +3167,11 @@
       <c r="AH1" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AU1" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
         <v>172</v>
@@ -3264,11 +3272,11 @@
       <c r="AH2" s="4">
         <v>31</v>
       </c>
-      <c r="AK2" s="4">
+      <c r="AU2" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
         <v>174</v>
@@ -3369,11 +3377,11 @@
       <c r="AH3" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="AK3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AU3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
       <c r="C4" s="3">
         <v>1</v>
       </c>
@@ -3470,14 +3478,14 @@
       <c r="AH4" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="AK4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AU4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>33</v>
       </c>
@@ -3577,14 +3585,52 @@
       <c r="AH6" s="4">
         <v>1</v>
       </c>
-      <c r="AK6" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI6" s="11" t="str">
+        <f>AH6&amp;AG6&amp;AF6&amp;AE6</f>
+        <v>1111</v>
+      </c>
+      <c r="AJ6" s="11" t="str">
+        <f>AD6&amp;AC6&amp;AB6&amp;AA6</f>
+        <v>0011</v>
+      </c>
+      <c r="AK6" s="11" t="str">
+        <f>Z6&amp;Y6&amp;X6&amp;W6</f>
+        <v>1110</v>
+      </c>
+      <c r="AL6" s="11" t="str">
+        <f>V6&amp;U6&amp;T6&amp;S6</f>
+        <v>1011</v>
+      </c>
+      <c r="AM6" s="11" t="str">
+        <f>R6&amp;Q6&amp;P6&amp;O6</f>
+        <v>1010</v>
+      </c>
+      <c r="AN6" s="11" t="str">
+        <f>N6&amp;M6&amp;L6&amp;K6</f>
+        <v>0000</v>
+      </c>
+      <c r="AO6" s="11" t="str">
+        <f>J6&amp;I6&amp;H6&amp;G6</f>
+        <v>0111</v>
+      </c>
+      <c r="AP6" s="11" t="str">
+        <f>F6&amp;E6&amp;D6&amp;C6</f>
+        <v>1111</v>
+      </c>
+      <c r="AQ6" s="11" t="str">
+        <f>BIN2HEX(AI6) &amp; BIN2HEX(AJ6) &amp; BIN2HEX(AK6) &amp; BIN2HEX(AL6) &amp; BIN2HEX(AM6) &amp; BIN2HEX(AN6) &amp; BIN2HEX(AO6) &amp; BIN2HEX(AP6)</f>
+        <v>F3EBA07F</v>
+      </c>
+      <c r="AU6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="G7" s="11"/>
+      <c r="AI7" s="11"/>
+    </row>
+    <row r="8" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>34</v>
       </c>
@@ -3684,11 +3730,47 @@
       <c r="AH8" s="4">
         <v>1</v>
       </c>
-      <c r="AK8" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI8" s="11" t="str">
+        <f t="shared" ref="AI8:AI71" si="0">AH8&amp;AG8&amp;AF8&amp;AE8</f>
+        <v>1111</v>
+      </c>
+      <c r="AJ8" s="11" t="str">
+        <f t="shared" ref="AJ8:AJ71" si="1">AD8&amp;AC8&amp;AB8&amp;AA8</f>
+        <v>0111</v>
+      </c>
+      <c r="AK8" s="11" t="str">
+        <f t="shared" ref="AK8:AK71" si="2">Z8&amp;Y8&amp;X8&amp;W8</f>
+        <v>1110</v>
+      </c>
+      <c r="AL8" s="11" t="str">
+        <f t="shared" ref="AL8:AL71" si="3">V8&amp;U8&amp;T8&amp;S8</f>
+        <v>1011</v>
+      </c>
+      <c r="AM8" s="11" t="str">
+        <f t="shared" ref="AM8:AM71" si="4">R8&amp;Q8&amp;P8&amp;O8</f>
+        <v>0110</v>
+      </c>
+      <c r="AN8" s="11" t="str">
+        <f t="shared" ref="AN8:AN71" si="5">N8&amp;M8&amp;L8&amp;K8</f>
+        <v>0000</v>
+      </c>
+      <c r="AO8" s="11" t="str">
+        <f t="shared" ref="AO8:AO71" si="6">J8&amp;I8&amp;H8&amp;G8</f>
+        <v>0111</v>
+      </c>
+      <c r="AP8" s="11" t="str">
+        <f t="shared" ref="AP8:AP71" si="7">F8&amp;E8&amp;D8&amp;C8</f>
+        <v>1111</v>
+      </c>
+      <c r="AQ8" s="11" t="str">
+        <f t="shared" ref="AQ7:AQ70" si="8">BIN2HEX(AI8) &amp; BIN2HEX(AJ8) &amp; BIN2HEX(AK8) &amp; BIN2HEX(AL8) &amp; BIN2HEX(AM8) &amp; BIN2HEX(AN8) &amp; BIN2HEX(AO8) &amp; BIN2HEX(AP8)</f>
+        <v>F7EB607F</v>
+      </c>
+      <c r="AU8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>35</v>
       </c>
@@ -3788,11 +3870,47 @@
       <c r="AH9" s="4">
         <v>1</v>
       </c>
-      <c r="AK9" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI9" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ9" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>0111</v>
+      </c>
+      <c r="AK9" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1110</v>
+      </c>
+      <c r="AL9" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1010</v>
+      </c>
+      <c r="AM9" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN9" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO9" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP9" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ9" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>F7EAE07F</v>
+      </c>
+      <c r="AU9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>36</v>
       </c>
@@ -3892,14 +4010,82 @@
       <c r="AH10" s="4">
         <v>1</v>
       </c>
-      <c r="AK10" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI10" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ10" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>0111</v>
+      </c>
+      <c r="AK10" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
+      <c r="AL10" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>0111</v>
+      </c>
+      <c r="AM10" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN10" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO10" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0011</v>
+      </c>
+      <c r="AP10" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ10" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>F7F7E03F</v>
+      </c>
+      <c r="AU10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI11" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AJ11" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AK11" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AL11" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AM11" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AN11" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AO11" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AP11" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>34</v>
       </c>
@@ -3999,11 +4185,47 @@
       <c r="AH12" s="4">
         <v>1</v>
       </c>
-      <c r="AK12" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI12" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ12" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>0111</v>
+      </c>
+      <c r="AK12" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1110</v>
+      </c>
+      <c r="AL12" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1011</v>
+      </c>
+      <c r="AM12" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>0110</v>
+      </c>
+      <c r="AN12" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO12" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP12" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ12" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>F7EB607F</v>
+      </c>
+      <c r="AU12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>35</v>
       </c>
@@ -4103,11 +4325,47 @@
       <c r="AH13" s="4">
         <v>1</v>
       </c>
-      <c r="AK13" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI13" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ13" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>0111</v>
+      </c>
+      <c r="AK13" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1110</v>
+      </c>
+      <c r="AL13" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1010</v>
+      </c>
+      <c r="AM13" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN13" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO13" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP13" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ13" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>F7EAE07F</v>
+      </c>
+      <c r="AU13" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>45</v>
       </c>
@@ -4207,14 +4465,82 @@
       <c r="AH14" s="4">
         <v>0</v>
       </c>
-      <c r="AK14" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI14" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>0000</v>
+      </c>
+      <c r="AJ14" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+      <c r="AK14" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
+      <c r="AL14" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>0111</v>
+      </c>
+      <c r="AM14" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN14" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0001</v>
+      </c>
+      <c r="AO14" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP14" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ14" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>0FF7E17F</v>
+      </c>
+      <c r="AU14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI15" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AJ15" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AK15" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AL15" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AM15" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AN15" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AO15" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AP15" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>37</v>
       </c>
@@ -4314,14 +4640,82 @@
       <c r="AH16" s="4">
         <v>1</v>
       </c>
-      <c r="AK16" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI16" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ16" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>0111</v>
+      </c>
+      <c r="AK16" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1110</v>
+      </c>
+      <c r="AL16" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1011</v>
+      </c>
+      <c r="AM16" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN16" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO16" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0011</v>
+      </c>
+      <c r="AP16" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ16" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>F7EBE03F</v>
+      </c>
+      <c r="AU16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI17" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AJ17" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AK17" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AL17" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AM17" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AN17" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AO17" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AP17" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>46</v>
       </c>
@@ -4421,11 +4815,47 @@
       <c r="AH18" s="4">
         <v>0</v>
       </c>
-      <c r="AK18" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI18" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>0001</v>
+      </c>
+      <c r="AJ18" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+      <c r="AK18" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
+      <c r="AL18" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1100</v>
+      </c>
+      <c r="AM18" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN18" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0001</v>
+      </c>
+      <c r="AO18" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0101</v>
+      </c>
+      <c r="AP18" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ18" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>1FFCE15F</v>
+      </c>
+      <c r="AU18" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>39</v>
       </c>
@@ -4525,14 +4955,86 @@
       <c r="AH19" s="4">
         <v>1</v>
       </c>
-      <c r="AK19" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:37" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AI19" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ19" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>0111</v>
+      </c>
+      <c r="AK19" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
+      <c r="AL19" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>0111</v>
+      </c>
+      <c r="AM19" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN19" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO19" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0011</v>
+      </c>
+      <c r="AP19" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ19" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>F7F7E03F</v>
+      </c>
+      <c r="AU19" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:47" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="2:37" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AI20" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AJ20" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AK20" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AL20" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AM20" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AN20" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AO20" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AP20" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AQ20" s="11"/>
+      <c r="AR20" s="11"/>
+      <c r="AS20" s="11"/>
+      <c r="AT20" s="11"/>
+    </row>
+    <row r="21" spans="2:47" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>46</v>
       </c>
@@ -4632,11 +5134,50 @@
       <c r="AH21" s="9">
         <v>0</v>
       </c>
-      <c r="AK21" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:37" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AI21" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>0001</v>
+      </c>
+      <c r="AJ21" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+      <c r="AK21" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
+      <c r="AL21" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1100</v>
+      </c>
+      <c r="AM21" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN21" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0001</v>
+      </c>
+      <c r="AO21" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0101</v>
+      </c>
+      <c r="AP21" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ21" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>1FFCE15F</v>
+      </c>
+      <c r="AR21" s="11"/>
+      <c r="AS21" s="11"/>
+      <c r="AT21" s="11"/>
+      <c r="AU21" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:47" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>225</v>
       </c>
@@ -4736,14 +5277,85 @@
       <c r="AH22" s="9">
         <v>0</v>
       </c>
-      <c r="AK22" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI22" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>0000</v>
+      </c>
+      <c r="AJ22" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+      <c r="AK22" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
+      <c r="AL22" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>0111</v>
+      </c>
+      <c r="AM22" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN22" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0001</v>
+      </c>
+      <c r="AO22" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP22" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ22" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>0FF7E17F</v>
+      </c>
+      <c r="AR22" s="11"/>
+      <c r="AS22" s="11"/>
+      <c r="AT22" s="11"/>
+      <c r="AU22" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI23" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AJ23" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AK23" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AL23" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AM23" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AN23" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AO23" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AP23" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
@@ -4843,11 +5455,47 @@
       <c r="AH24" s="4">
         <v>0</v>
       </c>
-      <c r="AK24" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI24" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>0001</v>
+      </c>
+      <c r="AJ24" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+      <c r="AK24" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
+      <c r="AL24" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1111</v>
+      </c>
+      <c r="AM24" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN24" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0001</v>
+      </c>
+      <c r="AO24" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP24" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1110</v>
+      </c>
+      <c r="AQ24" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>1FFFE17E</v>
+      </c>
+      <c r="AU24" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>40</v>
       </c>
@@ -4947,14 +5595,82 @@
       <c r="AH25" s="4">
         <v>0</v>
       </c>
-      <c r="AK25" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI25" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>0001</v>
+      </c>
+      <c r="AJ25" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+      <c r="AK25" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
+      <c r="AL25" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1111</v>
+      </c>
+      <c r="AM25" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN25" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0100</v>
+      </c>
+      <c r="AO25" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0001</v>
+      </c>
+      <c r="AP25" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ25" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>1FFFE41F</v>
+      </c>
+      <c r="AU25" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI26" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AJ26" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AK26" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AL26" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AM26" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AN26" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AO26" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AP26" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>43</v>
       </c>
@@ -5054,11 +5770,47 @@
       <c r="AH27" s="4">
         <v>0</v>
       </c>
-      <c r="AK27" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI27" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>0001</v>
+      </c>
+      <c r="AJ27" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+      <c r="AK27" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
+      <c r="AL27" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1111</v>
+      </c>
+      <c r="AM27" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN27" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0001</v>
+      </c>
+      <c r="AO27" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP27" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1110</v>
+      </c>
+      <c r="AQ27" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>1FFFE17E</v>
+      </c>
+      <c r="AU27" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>44</v>
       </c>
@@ -5158,14 +5910,82 @@
       <c r="AH28" s="4">
         <v>0</v>
       </c>
-      <c r="AK28" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI28" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>0001</v>
+      </c>
+      <c r="AJ28" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+      <c r="AK28" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
+      <c r="AL28" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1111</v>
+      </c>
+      <c r="AM28" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN28" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0100</v>
+      </c>
+      <c r="AO28" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0001</v>
+      </c>
+      <c r="AP28" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ28" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>1FFFE41F</v>
+      </c>
+      <c r="AU28" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B29" s="1"/>
-    </row>
-    <row r="30" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI29" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AJ29" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AK29" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AL29" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AM29" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AN29" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AO29" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AP29" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>34</v>
       </c>
@@ -5265,11 +6085,47 @@
       <c r="AH30" s="4">
         <v>1</v>
       </c>
-      <c r="AK30" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI30" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ30" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+      <c r="AK30" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1110</v>
+      </c>
+      <c r="AL30" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1011</v>
+      </c>
+      <c r="AM30" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>0110</v>
+      </c>
+      <c r="AN30" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO30" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP30" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ30" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>FFEB607F</v>
+      </c>
+      <c r="AU30" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>35</v>
       </c>
@@ -5369,11 +6225,47 @@
       <c r="AH31" s="4">
         <v>1</v>
       </c>
-      <c r="AK31" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI31" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ31" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+      <c r="AK31" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1110</v>
+      </c>
+      <c r="AL31" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1010</v>
+      </c>
+      <c r="AM31" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN31" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO31" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP31" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>FFEAE07F</v>
+      </c>
+      <c r="AU31" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>41</v>
       </c>
@@ -5473,14 +6365,82 @@
       <c r="AH32" s="4">
         <v>1</v>
       </c>
-      <c r="AK32" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI32" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ32" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1100</v>
+      </c>
+      <c r="AK32" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>0111</v>
+      </c>
+      <c r="AL32" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>0111</v>
+      </c>
+      <c r="AM32" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN32" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO32" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP32" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ32" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>FC77E07F</v>
+      </c>
+      <c r="AU32" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI33" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AJ33" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AK33" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AL33" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AM33" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AN33" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AO33" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AP33" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B34" s="7" t="s">
         <v>42</v>
       </c>
@@ -5580,11 +6540,47 @@
       <c r="AH34" s="4">
         <v>1</v>
       </c>
-      <c r="AK34" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI34" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ34" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>0111</v>
+      </c>
+      <c r="AK34" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1110</v>
+      </c>
+      <c r="AL34" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1010</v>
+      </c>
+      <c r="AM34" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>0110</v>
+      </c>
+      <c r="AN34" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO34" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP34" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1110</v>
+      </c>
+      <c r="AQ34" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>F7EA607E</v>
+      </c>
+      <c r="AU34" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>48</v>
       </c>
@@ -5684,11 +6680,47 @@
       <c r="AH35" s="4">
         <v>1</v>
       </c>
-      <c r="AK35" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI35" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1011</v>
+      </c>
+      <c r="AJ35" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+      <c r="AK35" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
+      <c r="AL35" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1111</v>
+      </c>
+      <c r="AM35" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN35" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO35" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP35" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>0111</v>
+      </c>
+      <c r="AQ35" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>BFFFE077</v>
+      </c>
+      <c r="AU35" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B36" s="7" t="s">
         <v>49</v>
       </c>
@@ -5788,11 +6820,47 @@
       <c r="AH36" s="4">
         <v>0</v>
       </c>
-      <c r="AK36" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI36" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>0001</v>
+      </c>
+      <c r="AJ36" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+      <c r="AK36" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
+      <c r="AL36" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1110</v>
+      </c>
+      <c r="AM36" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1111</v>
+      </c>
+      <c r="AN36" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>1110</v>
+      </c>
+      <c r="AO36" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>1111</v>
+      </c>
+      <c r="AP36" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ36" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>1FFEFEFF</v>
+      </c>
+      <c r="AU36" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>50</v>
       </c>
@@ -5892,11 +6960,47 @@
       <c r="AH37" s="4">
         <v>1</v>
       </c>
-      <c r="AK37" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI37" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1001</v>
+      </c>
+      <c r="AJ37" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+      <c r="AK37" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
+      <c r="AL37" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1111</v>
+      </c>
+      <c r="AM37" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN37" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO37" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP37" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>0011</v>
+      </c>
+      <c r="AQ37" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>9FFFE073</v>
+      </c>
+      <c r="AU37" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>51</v>
       </c>
@@ -5996,11 +7100,47 @@
       <c r="AH38" s="4">
         <v>0</v>
       </c>
-      <c r="AK38" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI38" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>0001</v>
+      </c>
+      <c r="AJ38" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+      <c r="AK38" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
+      <c r="AL38" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1111</v>
+      </c>
+      <c r="AM38" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>0111</v>
+      </c>
+      <c r="AN38" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0110</v>
+      </c>
+      <c r="AO38" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>1111</v>
+      </c>
+      <c r="AP38" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ38" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>1FFF76FF</v>
+      </c>
+      <c r="AU38" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>52</v>
       </c>
@@ -6100,14 +7240,82 @@
       <c r="AH39" s="4">
         <v>1</v>
       </c>
-      <c r="AK39" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI39" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ39" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1100</v>
+      </c>
+      <c r="AK39" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
+      <c r="AL39" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>0111</v>
+      </c>
+      <c r="AM39" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN39" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO39" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP39" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ39" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>FCF7E07F</v>
+      </c>
+      <c r="AU39" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B40" s="1"/>
-    </row>
-    <row r="41" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI40" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AJ40" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AK40" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AL40" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AM40" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AN40" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AO40" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AP40" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="1" t="s">
         <v>34</v>
@@ -6208,11 +7416,47 @@
       <c r="AH41" s="4">
         <v>1</v>
       </c>
-      <c r="AK41" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI41" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ41" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>0111</v>
+      </c>
+      <c r="AK41" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1110</v>
+      </c>
+      <c r="AL41" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1011</v>
+      </c>
+      <c r="AM41" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>0110</v>
+      </c>
+      <c r="AN41" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO41" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP41" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ41" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>F7EB607F</v>
+      </c>
+      <c r="AU41" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" s="1" t="s">
         <v>35</v>
@@ -6313,11 +7557,47 @@
       <c r="AH42" s="4">
         <v>1</v>
       </c>
-      <c r="AK42" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI42" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ42" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>0111</v>
+      </c>
+      <c r="AK42" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1110</v>
+      </c>
+      <c r="AL42" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1010</v>
+      </c>
+      <c r="AM42" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN42" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO42" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP42" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ42" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>F7EAE07F</v>
+      </c>
+      <c r="AU42" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>53</v>
       </c>
@@ -6417,11 +7697,47 @@
       <c r="AH43" s="4">
         <v>0</v>
       </c>
-      <c r="AK43" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI43" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>0100</v>
+      </c>
+      <c r="AJ43" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+      <c r="AK43" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1101</v>
+      </c>
+      <c r="AL43" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>0011</v>
+      </c>
+      <c r="AM43" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN43" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO43" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP43" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ43" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>4FD3E07F</v>
+      </c>
+      <c r="AU43" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
         <v>57</v>
       </c>
@@ -6521,11 +7837,47 @@
       <c r="AH44" s="4">
         <v>0</v>
       </c>
-      <c r="AK44" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI44" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>0010</v>
+      </c>
+      <c r="AJ44" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+      <c r="AK44" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1101</v>
+      </c>
+      <c r="AL44" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>0011</v>
+      </c>
+      <c r="AM44" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN44" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO44" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP44" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ44" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>2FD3E07F</v>
+      </c>
+      <c r="AU44" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
         <v>41</v>
       </c>
@@ -6625,14 +7977,82 @@
       <c r="AH45" s="4">
         <v>1</v>
       </c>
-      <c r="AK45" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI45" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ45" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1100</v>
+      </c>
+      <c r="AK45" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>0111</v>
+      </c>
+      <c r="AL45" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>0111</v>
+      </c>
+      <c r="AM45" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN45" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO45" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP45" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ45" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>FC77E07F</v>
+      </c>
+      <c r="AU45" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B46" s="1"/>
-    </row>
-    <row r="47" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI46" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AJ46" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AK46" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AL46" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AM46" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AN46" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AO46" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AP46" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
         <v>56</v>
       </c>
@@ -6732,11 +8152,47 @@
       <c r="AH47" s="4">
         <v>1</v>
       </c>
-      <c r="AK47" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AI47" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ47" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+      <c r="AK47" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1011</v>
+      </c>
+      <c r="AL47" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1111</v>
+      </c>
+      <c r="AM47" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN47" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO47" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP47" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ47" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>FFBFE07F</v>
+      </c>
+      <c r="AU47" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
         <v>58</v>
       </c>
@@ -6836,11 +8292,47 @@
       <c r="AH48" s="4">
         <v>1</v>
       </c>
-      <c r="AK48" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI48" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ48" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>0111</v>
+      </c>
+      <c r="AK48" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1011</v>
+      </c>
+      <c r="AL48" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>0011</v>
+      </c>
+      <c r="AM48" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>0110</v>
+      </c>
+      <c r="AN48" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO48" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP48" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ48" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>F7B3607F</v>
+      </c>
+      <c r="AU48" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
         <v>59</v>
       </c>
@@ -6940,11 +8432,47 @@
       <c r="AH49" s="4">
         <v>1</v>
       </c>
-      <c r="AK49" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI49" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ49" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>0111</v>
+      </c>
+      <c r="AK49" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
+      <c r="AL49" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>0010</v>
+      </c>
+      <c r="AM49" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN49" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO49" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP49" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ49" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>F7F2E07F</v>
+      </c>
+      <c r="AU49" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
         <v>41</v>
       </c>
@@ -7044,14 +8572,82 @@
       <c r="AH50" s="4">
         <v>1</v>
       </c>
-      <c r="AK50" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI50" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ50" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1100</v>
+      </c>
+      <c r="AK50" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>0111</v>
+      </c>
+      <c r="AL50" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>0111</v>
+      </c>
+      <c r="AM50" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN50" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO50" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP50" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ50" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>FC77E07F</v>
+      </c>
+      <c r="AU50" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B51" s="1"/>
-    </row>
-    <row r="52" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI51" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AJ51" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AK51" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AL51" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AM51" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AN51" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AO51" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AP51" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
         <v>60</v>
       </c>
@@ -7151,14 +8747,82 @@
       <c r="AH52" s="4">
         <v>0</v>
       </c>
-      <c r="AK52" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI52" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>0000</v>
+      </c>
+      <c r="AJ52" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+      <c r="AK52" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1101</v>
+      </c>
+      <c r="AL52" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>0011</v>
+      </c>
+      <c r="AM52" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN52" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0001</v>
+      </c>
+      <c r="AO52" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP52" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ52" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>0FD3E17F</v>
+      </c>
+      <c r="AU52" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B53" s="1"/>
-    </row>
-    <row r="54" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI53" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AJ53" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AK53" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AL53" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AM53" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AN53" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AO53" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AP53" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
         <v>61</v>
       </c>
@@ -7258,11 +8922,47 @@
       <c r="AH54" s="4">
         <v>1</v>
       </c>
-      <c r="AK54" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI54" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ54" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+      <c r="AK54" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1011</v>
+      </c>
+      <c r="AL54" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1111</v>
+      </c>
+      <c r="AM54" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN54" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO54" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP54" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ54" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>FFBFE07F</v>
+      </c>
+      <c r="AU54" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B55" s="1" t="s">
         <v>62</v>
       </c>
@@ -7362,14 +9062,82 @@
       <c r="AH55" s="4">
         <v>1</v>
       </c>
-      <c r="AK55" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI55" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ55" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>0111</v>
+      </c>
+      <c r="AK55" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
+      <c r="AL55" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>0011</v>
+      </c>
+      <c r="AM55" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN55" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO55" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0011</v>
+      </c>
+      <c r="AP55" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ55" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>F7F3E03F</v>
+      </c>
+      <c r="AU55" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B56" s="1"/>
-    </row>
-    <row r="57" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI56" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AJ56" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AK56" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AL56" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AM56" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AN56" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AO56" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AP56" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B57" s="1" t="s">
         <v>65</v>
       </c>
@@ -7469,11 +9237,47 @@
       <c r="AH57" s="4">
         <v>0</v>
       </c>
-      <c r="AK57" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI57" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>0001</v>
+      </c>
+      <c r="AJ57" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+      <c r="AK57" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
+      <c r="AL57" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1100</v>
+      </c>
+      <c r="AM57" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN57" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0001</v>
+      </c>
+      <c r="AO57" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0101</v>
+      </c>
+      <c r="AP57" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ57" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>1FFCE15F</v>
+      </c>
+      <c r="AU57" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B58" s="1" t="s">
         <v>63</v>
       </c>
@@ -7573,11 +9377,47 @@
       <c r="AH58" s="4">
         <v>1</v>
       </c>
-      <c r="AK58" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI58" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ58" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>0111</v>
+      </c>
+      <c r="AK58" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
+      <c r="AL58" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>0111</v>
+      </c>
+      <c r="AM58" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN58" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO58" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP58" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1110</v>
+      </c>
+      <c r="AQ58" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>F7F7E07E</v>
+      </c>
+      <c r="AU58" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B59" s="1" t="s">
         <v>64</v>
       </c>
@@ -7677,14 +9517,82 @@
       <c r="AH59" s="4">
         <v>0</v>
       </c>
-      <c r="AK59" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI59" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>0001</v>
+      </c>
+      <c r="AJ59" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+      <c r="AK59" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
+      <c r="AL59" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1111</v>
+      </c>
+      <c r="AM59" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN59" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>1110</v>
+      </c>
+      <c r="AO59" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0011</v>
+      </c>
+      <c r="AP59" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ59" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>1FFFEE3F</v>
+      </c>
+      <c r="AU59" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B60" s="1"/>
-    </row>
-    <row r="61" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI60" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AJ60" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AK60" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AL60" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AM60" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AN60" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AO60" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AP60" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B61" s="1" t="s">
         <v>66</v>
       </c>
@@ -7784,11 +9692,47 @@
       <c r="AH61" s="4">
         <v>1</v>
       </c>
-      <c r="AK61" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI61" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ61" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>0111</v>
+      </c>
+      <c r="AK61" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1110</v>
+      </c>
+      <c r="AL61" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1011</v>
+      </c>
+      <c r="AM61" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN61" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO61" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP61" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1110</v>
+      </c>
+      <c r="AQ61" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>F7EBE07E</v>
+      </c>
+      <c r="AU61" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B62" s="1" t="s">
         <v>67</v>
       </c>
@@ -7888,14 +9832,82 @@
       <c r="AH62" s="4">
         <v>0</v>
       </c>
-      <c r="AK62" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI62" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>0001</v>
+      </c>
+      <c r="AJ62" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+      <c r="AK62" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
+      <c r="AL62" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1111</v>
+      </c>
+      <c r="AM62" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN62" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0010</v>
+      </c>
+      <c r="AO62" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0011</v>
+      </c>
+      <c r="AP62" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ62" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>1FFFE23F</v>
+      </c>
+      <c r="AU62" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B63" s="1"/>
-    </row>
-    <row r="64" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI63" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AJ63" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AK63" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AL63" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AM63" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AN63" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AO63" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AP63" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B64" s="1" t="s">
         <v>34</v>
       </c>
@@ -7995,11 +10007,47 @@
       <c r="AH64" s="4">
         <v>1</v>
       </c>
-      <c r="AK64" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI64" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ64" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>0111</v>
+      </c>
+      <c r="AK64" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1110</v>
+      </c>
+      <c r="AL64" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1011</v>
+      </c>
+      <c r="AM64" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>0110</v>
+      </c>
+      <c r="AN64" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO64" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP64" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ64" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>F7EB607F</v>
+      </c>
+      <c r="AU64" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B65" s="1" t="s">
         <v>68</v>
       </c>
@@ -8099,11 +10147,47 @@
       <c r="AH65" s="4">
         <v>1</v>
       </c>
-      <c r="AK65" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI65" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ65" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>0111</v>
+      </c>
+      <c r="AK65" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1110</v>
+      </c>
+      <c r="AL65" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1010</v>
+      </c>
+      <c r="AM65" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN65" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO65" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP65" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ65" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>F7EAE07F</v>
+      </c>
+      <c r="AU65" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B66" s="1" t="s">
         <v>69</v>
       </c>
@@ -8203,11 +10287,47 @@
       <c r="AH66" s="4">
         <v>1</v>
       </c>
-      <c r="AK66" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI66" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ66" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>0111</v>
+      </c>
+      <c r="AK66" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
+      <c r="AL66" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>0111</v>
+      </c>
+      <c r="AM66" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN66" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO66" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP66" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>0011</v>
+      </c>
+      <c r="AQ66" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>F7F7E073</v>
+      </c>
+      <c r="AU66" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
         <v>70</v>
       </c>
@@ -8307,14 +10427,82 @@
       <c r="AH67" s="4">
         <v>0</v>
       </c>
-      <c r="AK67" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI67" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>0000</v>
+      </c>
+      <c r="AJ67" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+      <c r="AK67" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
+      <c r="AL67" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>0111</v>
+      </c>
+      <c r="AM67" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1111</v>
+      </c>
+      <c r="AN67" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>1110</v>
+      </c>
+      <c r="AO67" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>1111</v>
+      </c>
+      <c r="AP67" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ67" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>0FF7FEFF</v>
+      </c>
+      <c r="AU67" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B68" s="1"/>
-    </row>
-    <row r="69" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI68" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AJ68" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AK68" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AL68" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="AM68" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AN68" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AO68" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AP68" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B69" s="1" t="s">
         <v>42</v>
       </c>
@@ -8414,11 +10602,47 @@
       <c r="AH69" s="4">
         <v>1</v>
       </c>
-      <c r="AK69" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI69" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ69" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>0111</v>
+      </c>
+      <c r="AK69" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1110</v>
+      </c>
+      <c r="AL69" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1010</v>
+      </c>
+      <c r="AM69" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>0110</v>
+      </c>
+      <c r="AN69" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO69" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP69" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1110</v>
+      </c>
+      <c r="AQ69" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>F7EA607E</v>
+      </c>
+      <c r="AU69" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B70" s="1" t="s">
         <v>48</v>
       </c>
@@ -8518,11 +10742,47 @@
       <c r="AH70" s="4">
         <v>1</v>
       </c>
-      <c r="AK70" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI70" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1011</v>
+      </c>
+      <c r="AJ70" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+      <c r="AK70" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
+      <c r="AL70" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1111</v>
+      </c>
+      <c r="AM70" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1110</v>
+      </c>
+      <c r="AN70" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>0000</v>
+      </c>
+      <c r="AO70" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>0111</v>
+      </c>
+      <c r="AP70" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>0111</v>
+      </c>
+      <c r="AQ70" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>BFFFE077</v>
+      </c>
+      <c r="AU70" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B71" s="7" t="s">
         <v>49</v>
       </c>
@@ -8622,11 +10882,47 @@
       <c r="AH71" s="4">
         <v>0</v>
       </c>
-      <c r="AK71" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI71" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>0001</v>
+      </c>
+      <c r="AJ71" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1111</v>
+      </c>
+      <c r="AK71" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
+      <c r="AL71" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1110</v>
+      </c>
+      <c r="AM71" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>1111</v>
+      </c>
+      <c r="AN71" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v>1110</v>
+      </c>
+      <c r="AO71" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v>1111</v>
+      </c>
+      <c r="AP71" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ71" s="11" t="str">
+        <f t="shared" ref="AQ71:AQ85" si="9">BIN2HEX(AI71) &amp; BIN2HEX(AJ71) &amp; BIN2HEX(AK71) &amp; BIN2HEX(AL71) &amp; BIN2HEX(AM71) &amp; BIN2HEX(AN71) &amp; BIN2HEX(AO71) &amp; BIN2HEX(AP71)</f>
+        <v>1FFEFEFF</v>
+      </c>
+      <c r="AU71" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B72" s="1" t="s">
         <v>50</v>
       </c>
@@ -8726,11 +11022,47 @@
       <c r="AH72" s="4">
         <v>1</v>
       </c>
-      <c r="AK72" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI72" s="11" t="str">
+        <f t="shared" ref="AI72:AI85" si="10">AH72&amp;AG72&amp;AF72&amp;AE72</f>
+        <v>1001</v>
+      </c>
+      <c r="AJ72" s="11" t="str">
+        <f t="shared" ref="AJ72:AJ85" si="11">AD72&amp;AC72&amp;AB72&amp;AA72</f>
+        <v>1111</v>
+      </c>
+      <c r="AK72" s="11" t="str">
+        <f t="shared" ref="AK72:AK85" si="12">Z72&amp;Y72&amp;X72&amp;W72</f>
+        <v>1111</v>
+      </c>
+      <c r="AL72" s="11" t="str">
+        <f t="shared" ref="AL72:AL85" si="13">V72&amp;U72&amp;T72&amp;S72</f>
+        <v>1111</v>
+      </c>
+      <c r="AM72" s="11" t="str">
+        <f t="shared" ref="AM72:AM85" si="14">R72&amp;Q72&amp;P72&amp;O72</f>
+        <v>1110</v>
+      </c>
+      <c r="AN72" s="11" t="str">
+        <f t="shared" ref="AN72:AN85" si="15">N72&amp;M72&amp;L72&amp;K72</f>
+        <v>0000</v>
+      </c>
+      <c r="AO72" s="11" t="str">
+        <f t="shared" ref="AO72:AO85" si="16">J72&amp;I72&amp;H72&amp;G72</f>
+        <v>0111</v>
+      </c>
+      <c r="AP72" s="11" t="str">
+        <f t="shared" ref="AP72:AP85" si="17">F72&amp;E72&amp;D72&amp;C72</f>
+        <v>0011</v>
+      </c>
+      <c r="AQ72" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>9FFFE073</v>
+      </c>
+      <c r="AU72" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B73" s="1" t="s">
         <v>51</v>
       </c>
@@ -8830,11 +11162,47 @@
       <c r="AH73" s="4">
         <v>0</v>
       </c>
-      <c r="AK73" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI73" s="11" t="str">
+        <f t="shared" si="10"/>
+        <v>0001</v>
+      </c>
+      <c r="AJ73" s="11" t="str">
+        <f t="shared" si="11"/>
+        <v>1111</v>
+      </c>
+      <c r="AK73" s="11" t="str">
+        <f t="shared" si="12"/>
+        <v>1111</v>
+      </c>
+      <c r="AL73" s="11" t="str">
+        <f t="shared" si="13"/>
+        <v>1111</v>
+      </c>
+      <c r="AM73" s="11" t="str">
+        <f t="shared" si="14"/>
+        <v>0111</v>
+      </c>
+      <c r="AN73" s="11" t="str">
+        <f t="shared" si="15"/>
+        <v>0110</v>
+      </c>
+      <c r="AO73" s="11" t="str">
+        <f t="shared" si="16"/>
+        <v>1111</v>
+      </c>
+      <c r="AP73" s="11" t="str">
+        <f t="shared" si="17"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ73" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>1FFF76FF</v>
+      </c>
+      <c r="AU73" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B74" s="1" t="s">
         <v>71</v>
       </c>
@@ -8934,14 +11302,82 @@
       <c r="AH74" s="4">
         <v>1</v>
       </c>
-      <c r="AK74" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI74" s="11" t="str">
+        <f t="shared" si="10"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ74" s="11" t="str">
+        <f t="shared" si="11"/>
+        <v>1101</v>
+      </c>
+      <c r="AK74" s="11" t="str">
+        <f t="shared" si="12"/>
+        <v>1111</v>
+      </c>
+      <c r="AL74" s="11" t="str">
+        <f t="shared" si="13"/>
+        <v>1111</v>
+      </c>
+      <c r="AM74" s="11" t="str">
+        <f t="shared" si="14"/>
+        <v>1110</v>
+      </c>
+      <c r="AN74" s="11" t="str">
+        <f t="shared" si="15"/>
+        <v>0000</v>
+      </c>
+      <c r="AO74" s="11" t="str">
+        <f t="shared" si="16"/>
+        <v>0111</v>
+      </c>
+      <c r="AP74" s="11" t="str">
+        <f t="shared" si="17"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ74" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>FDFFE07F</v>
+      </c>
+      <c r="AU74" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B75" s="1"/>
-    </row>
-    <row r="76" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI75" s="11" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="AJ75" s="11" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AK75" s="11" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="AL75" s="11" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="AM75" s="11" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="AN75" s="11" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="AO75" s="11" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="AP75" s="11" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B76" s="1" t="s">
         <v>42</v>
       </c>
@@ -9041,11 +11477,47 @@
       <c r="AH76" s="4">
         <v>1</v>
       </c>
-      <c r="AK76" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI76" s="11" t="str">
+        <f t="shared" si="10"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ76" s="11" t="str">
+        <f t="shared" si="11"/>
+        <v>0111</v>
+      </c>
+      <c r="AK76" s="11" t="str">
+        <f t="shared" si="12"/>
+        <v>1110</v>
+      </c>
+      <c r="AL76" s="11" t="str">
+        <f t="shared" si="13"/>
+        <v>1010</v>
+      </c>
+      <c r="AM76" s="11" t="str">
+        <f t="shared" si="14"/>
+        <v>0110</v>
+      </c>
+      <c r="AN76" s="11" t="str">
+        <f t="shared" si="15"/>
+        <v>0000</v>
+      </c>
+      <c r="AO76" s="11" t="str">
+        <f t="shared" si="16"/>
+        <v>0111</v>
+      </c>
+      <c r="AP76" s="11" t="str">
+        <f t="shared" si="17"/>
+        <v>1110</v>
+      </c>
+      <c r="AQ76" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>F7EA607E</v>
+      </c>
+      <c r="AU76" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B77" s="1" t="s">
         <v>48</v>
       </c>
@@ -9145,11 +11617,47 @@
       <c r="AH77" s="4">
         <v>1</v>
       </c>
-      <c r="AK77" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI77" s="11" t="str">
+        <f t="shared" si="10"/>
+        <v>1011</v>
+      </c>
+      <c r="AJ77" s="11" t="str">
+        <f t="shared" si="11"/>
+        <v>1111</v>
+      </c>
+      <c r="AK77" s="11" t="str">
+        <f t="shared" si="12"/>
+        <v>1111</v>
+      </c>
+      <c r="AL77" s="11" t="str">
+        <f t="shared" si="13"/>
+        <v>1111</v>
+      </c>
+      <c r="AM77" s="11" t="str">
+        <f t="shared" si="14"/>
+        <v>1110</v>
+      </c>
+      <c r="AN77" s="11" t="str">
+        <f t="shared" si="15"/>
+        <v>0000</v>
+      </c>
+      <c r="AO77" s="11" t="str">
+        <f t="shared" si="16"/>
+        <v>0111</v>
+      </c>
+      <c r="AP77" s="11" t="str">
+        <f t="shared" si="17"/>
+        <v>0111</v>
+      </c>
+      <c r="AQ77" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>BFFFE077</v>
+      </c>
+      <c r="AU77" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B78" s="7" t="s">
         <v>49</v>
       </c>
@@ -9249,11 +11757,47 @@
       <c r="AH78" s="4">
         <v>0</v>
       </c>
-      <c r="AK78" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI78" s="11" t="str">
+        <f t="shared" si="10"/>
+        <v>0001</v>
+      </c>
+      <c r="AJ78" s="11" t="str">
+        <f t="shared" si="11"/>
+        <v>1111</v>
+      </c>
+      <c r="AK78" s="11" t="str">
+        <f t="shared" si="12"/>
+        <v>1111</v>
+      </c>
+      <c r="AL78" s="11" t="str">
+        <f t="shared" si="13"/>
+        <v>1110</v>
+      </c>
+      <c r="AM78" s="11" t="str">
+        <f t="shared" si="14"/>
+        <v>1111</v>
+      </c>
+      <c r="AN78" s="11" t="str">
+        <f t="shared" si="15"/>
+        <v>1110</v>
+      </c>
+      <c r="AO78" s="11" t="str">
+        <f t="shared" si="16"/>
+        <v>1111</v>
+      </c>
+      <c r="AP78" s="11" t="str">
+        <f t="shared" si="17"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ78" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>1FFEFEFF</v>
+      </c>
+      <c r="AU78" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B79" s="1" t="s">
         <v>50</v>
       </c>
@@ -9353,11 +11897,47 @@
       <c r="AH79" s="4">
         <v>1</v>
       </c>
-      <c r="AK79" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI79" s="11" t="str">
+        <f t="shared" si="10"/>
+        <v>1001</v>
+      </c>
+      <c r="AJ79" s="11" t="str">
+        <f t="shared" si="11"/>
+        <v>1111</v>
+      </c>
+      <c r="AK79" s="11" t="str">
+        <f t="shared" si="12"/>
+        <v>1111</v>
+      </c>
+      <c r="AL79" s="11" t="str">
+        <f t="shared" si="13"/>
+        <v>1111</v>
+      </c>
+      <c r="AM79" s="11" t="str">
+        <f t="shared" si="14"/>
+        <v>1110</v>
+      </c>
+      <c r="AN79" s="11" t="str">
+        <f t="shared" si="15"/>
+        <v>0000</v>
+      </c>
+      <c r="AO79" s="11" t="str">
+        <f t="shared" si="16"/>
+        <v>0111</v>
+      </c>
+      <c r="AP79" s="11" t="str">
+        <f t="shared" si="17"/>
+        <v>0011</v>
+      </c>
+      <c r="AQ79" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>9FFFE073</v>
+      </c>
+      <c r="AU79" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B80" s="1" t="s">
         <v>51</v>
       </c>
@@ -9457,11 +12037,47 @@
       <c r="AH80" s="4">
         <v>0</v>
       </c>
-      <c r="AK80" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI80" s="11" t="str">
+        <f t="shared" si="10"/>
+        <v>0001</v>
+      </c>
+      <c r="AJ80" s="11" t="str">
+        <f t="shared" si="11"/>
+        <v>1111</v>
+      </c>
+      <c r="AK80" s="11" t="str">
+        <f t="shared" si="12"/>
+        <v>1111</v>
+      </c>
+      <c r="AL80" s="11" t="str">
+        <f t="shared" si="13"/>
+        <v>1111</v>
+      </c>
+      <c r="AM80" s="11" t="str">
+        <f t="shared" si="14"/>
+        <v>0111</v>
+      </c>
+      <c r="AN80" s="11" t="str">
+        <f t="shared" si="15"/>
+        <v>0110</v>
+      </c>
+      <c r="AO80" s="11" t="str">
+        <f t="shared" si="16"/>
+        <v>1111</v>
+      </c>
+      <c r="AP80" s="11" t="str">
+        <f t="shared" si="17"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ80" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>1FFF76FF</v>
+      </c>
+      <c r="AU80" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B81" s="1" t="s">
         <v>72</v>
       </c>
@@ -9561,14 +12177,82 @@
       <c r="AH81" s="4">
         <v>1</v>
       </c>
-      <c r="AK81" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI81" s="11" t="str">
+        <f t="shared" si="10"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ81" s="11" t="str">
+        <f t="shared" si="11"/>
+        <v>1101</v>
+      </c>
+      <c r="AK81" s="11" t="str">
+        <f t="shared" si="12"/>
+        <v>0111</v>
+      </c>
+      <c r="AL81" s="11" t="str">
+        <f t="shared" si="13"/>
+        <v>1111</v>
+      </c>
+      <c r="AM81" s="11" t="str">
+        <f t="shared" si="14"/>
+        <v>1110</v>
+      </c>
+      <c r="AN81" s="11" t="str">
+        <f t="shared" si="15"/>
+        <v>0000</v>
+      </c>
+      <c r="AO81" s="11" t="str">
+        <f t="shared" si="16"/>
+        <v>0111</v>
+      </c>
+      <c r="AP81" s="11" t="str">
+        <f t="shared" si="17"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ81" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>FD7FE07F</v>
+      </c>
+      <c r="AU81" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B82" s="1"/>
-    </row>
-    <row r="83" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI82" s="11" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="AJ82" s="11" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AK82" s="11" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="AL82" s="11" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="AM82" s="11" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="AN82" s="11" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="AO82" s="11" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="AP82" s="11" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B83" s="1" t="s">
         <v>73</v>
       </c>
@@ -9668,11 +12352,47 @@
       <c r="AH83" s="4">
         <v>0</v>
       </c>
-      <c r="AK83" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI83" s="11" t="str">
+        <f t="shared" si="10"/>
+        <v>0001</v>
+      </c>
+      <c r="AJ83" s="11" t="str">
+        <f t="shared" si="11"/>
+        <v>1111</v>
+      </c>
+      <c r="AK83" s="11" t="str">
+        <f t="shared" si="12"/>
+        <v>1111</v>
+      </c>
+      <c r="AL83" s="11" t="str">
+        <f t="shared" si="13"/>
+        <v>1111</v>
+      </c>
+      <c r="AM83" s="11" t="str">
+        <f t="shared" si="14"/>
+        <v>1110</v>
+      </c>
+      <c r="AN83" s="11" t="str">
+        <f t="shared" si="15"/>
+        <v>0001</v>
+      </c>
+      <c r="AO83" s="11" t="str">
+        <f t="shared" si="16"/>
+        <v>0111</v>
+      </c>
+      <c r="AP83" s="11" t="str">
+        <f t="shared" si="17"/>
+        <v>1110</v>
+      </c>
+      <c r="AQ83" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>1FFFE17E</v>
+      </c>
+      <c r="AU83" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B84" s="1" t="s">
         <v>213</v>
       </c>
@@ -9772,11 +12492,47 @@
       <c r="AH84" s="4">
         <v>1</v>
       </c>
-      <c r="AK84" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="AI84" s="11" t="str">
+        <f t="shared" si="10"/>
+        <v>1111</v>
+      </c>
+      <c r="AJ84" s="11" t="str">
+        <f t="shared" si="11"/>
+        <v>1111</v>
+      </c>
+      <c r="AK84" s="11" t="str">
+        <f t="shared" si="12"/>
+        <v>1111</v>
+      </c>
+      <c r="AL84" s="11" t="str">
+        <f t="shared" si="13"/>
+        <v>1111</v>
+      </c>
+      <c r="AM84" s="11" t="str">
+        <f t="shared" si="14"/>
+        <v>1110</v>
+      </c>
+      <c r="AN84" s="11" t="str">
+        <f t="shared" si="15"/>
+        <v>0000</v>
+      </c>
+      <c r="AO84" s="11" t="str">
+        <f t="shared" si="16"/>
+        <v>0111</v>
+      </c>
+      <c r="AP84" s="11" t="str">
+        <f t="shared" si="17"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ84" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>FFFFE07F</v>
+      </c>
+      <c r="AU84" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B85" s="1" t="s">
         <v>75</v>
       </c>
@@ -9834,11 +12590,11 @@
       <c r="T85" s="4">
         <v>1</v>
       </c>
-      <c r="U85" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="V85" s="4" t="s">
-        <v>194</v>
+      <c r="U85" s="4">
+        <v>1</v>
+      </c>
+      <c r="V85" s="4">
+        <v>1</v>
       </c>
       <c r="W85" s="4">
         <v>1</v>
@@ -9849,14 +12605,14 @@
       <c r="Y85" s="4">
         <v>1</v>
       </c>
-      <c r="Z85" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="AA85" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="AB85" s="4" t="s">
-        <v>194</v>
+      <c r="Z85" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA85" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB85" s="4">
+        <v>1</v>
       </c>
       <c r="AC85" s="4">
         <v>1</v>
@@ -9876,7 +12632,43 @@
       <c r="AH85" s="4">
         <v>0</v>
       </c>
-      <c r="AK85" s="4">
+      <c r="AI85" s="11" t="str">
+        <f t="shared" si="10"/>
+        <v>0001</v>
+      </c>
+      <c r="AJ85" s="11" t="str">
+        <f t="shared" si="11"/>
+        <v>1111</v>
+      </c>
+      <c r="AK85" s="11" t="str">
+        <f t="shared" si="12"/>
+        <v>1111</v>
+      </c>
+      <c r="AL85" s="11" t="str">
+        <f t="shared" si="13"/>
+        <v>1111</v>
+      </c>
+      <c r="AM85" s="11" t="str">
+        <f t="shared" si="14"/>
+        <v>1110</v>
+      </c>
+      <c r="AN85" s="11" t="str">
+        <f t="shared" si="15"/>
+        <v>0000</v>
+      </c>
+      <c r="AO85" s="11" t="str">
+        <f t="shared" si="16"/>
+        <v>0011</v>
+      </c>
+      <c r="AP85" s="11" t="str">
+        <f t="shared" si="17"/>
+        <v>1111</v>
+      </c>
+      <c r="AQ85" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>1FFFE03F</v>
+      </c>
+      <c r="AU85" s="4">
         <v>0</v>
       </c>
     </row>

</xml_diff>